<commit_message>
fixes enumeration issue in releasefish xlsx
</commit_message>
<xml_diff>
--- a/data-raw/metadata/camp_releasefish_metadata.xlsx
+++ b/data-raw/metadata/camp_releasefish_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/jpe-knights-edi/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6165223E-F2C5-FB4F-A468-A7D47BCC0E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5612B92E-28B8-6D49-A8FC-EDBD07A00D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="73040" yWindow="-11100" windowWidth="30240" windowHeight="17300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -147,6 +147,9 @@
   <si>
     <t>count of fish</t>
   </si>
+  <si>
+    <t>Feather River RST Program</t>
+  </si>
 </sst>
 </file>
 
@@ -163,17 +166,20 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -216,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -241,6 +247,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,9 +465,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -28484,8 +28491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -28531,9 +28538,15 @@
       <c r="Z1" s="9"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="A2" s="12">
+        <v>2</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>13</v>
+      </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>

</xml_diff>